<commit_message>
feat: Added hanning frame correction (though it doesnt make a diifference due to ratio cancellation but still good coding practise. ) Additionally added a early data training with vad guidance for a noise estimation model.
</commit_message>
<xml_diff>
--- a/Random/Matlab2025Files/SS/selected_algorithm_metrics.xlsx
+++ b/Random/Matlab2025Files/SS/selected_algorithm_metrics.xlsx
@@ -342,67 +342,67 @@
         <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>10.341197750382351</v>
+        <v>10.341197727994746</v>
       </c>
       <c r="D3" s="0">
-        <v>5.2788046228066285</v>
+        <v>5.2788045858864781</v>
       </c>
       <c r="E3" s="0">
-        <v>60.071444001870084</v>
+        <v>60.07144404456659</v>
       </c>
       <c r="F3" s="0">
-        <v>0.94200352869294701</v>
+        <v>0.94200362288809669</v>
       </c>
       <c r="G3" s="0">
-        <v>2.1157395308514855</v>
+        <v>2.1157402048391329</v>
       </c>
       <c r="H3" s="0">
-        <v>5.6067456421604769</v>
+        <v>5.6067460485695824</v>
       </c>
       <c r="I3" s="0">
-        <v>5.68604408941603</v>
+        <v>5.6860435400959028</v>
       </c>
       <c r="J3" s="0">
-        <v>2.6095815994641409</v>
+        <v>2.6095815800558269</v>
       </c>
       <c r="K3" s="0">
-        <v>1.854792974158173</v>
+        <v>1.8547929787418278</v>
       </c>
       <c r="L3" s="0">
-        <v>2.0655389211605488</v>
+        <v>2.065538909215618</v>
       </c>
       <c r="M3" s="0">
-        <v>2.6172868271178271</v>
+        <v>2.6172867754110838</v>
       </c>
       <c r="N3" s="0">
-        <v>2.6643349445739917</v>
+        <v>2.6643349590082228</v>
       </c>
       <c r="O3" s="0">
-        <v>2.009741253538027</v>
+        <v>2.0097412581674696</v>
       </c>
       <c r="P3" s="0">
-        <v>1.4187802082701539</v>
+        <v>1.4187802051127576</v>
       </c>
       <c r="Q3" s="0">
-        <v>2.3455159214659549</v>
+        <v>2.3455158234006284</v>
       </c>
       <c r="R3" s="0">
-        <v>2.2242415227768597</v>
+        <v>2.2242415186427795</v>
       </c>
       <c r="S3" s="0">
-        <v>1.7870162486343659</v>
+        <v>1.7870161981379074</v>
       </c>
       <c r="T3" s="0">
-        <v>0.91821799085166289</v>
+        <v>0.91821799776110646</v>
       </c>
       <c r="U3" s="0">
-        <v>0.87686995606187712</v>
+        <v>0.87686995567658122</v>
       </c>
       <c r="V3" s="0">
-        <v>0.6364707912539509</v>
+        <v>0.63647078999474294</v>
       </c>
       <c r="W3" s="0">
-        <v>0.13740675778929057</v>
+        <v>0.13740675665473895</v>
       </c>
       <c r="X3" s="0">
         <v>0.23571173354711331</v>
@@ -416,67 +416,67 @@
         <v>8</v>
       </c>
       <c r="C4" s="0">
-        <v>7.673406372177908</v>
+        <v>7.6734063747941512</v>
       </c>
       <c r="D4" s="0">
-        <v>2.1524493440773411</v>
+        <v>2.1524493523483641</v>
       </c>
       <c r="E4" s="0">
-        <v>88.185983819428614</v>
+        <v>88.18598373657359</v>
       </c>
       <c r="F4" s="0">
-        <v>1.2583780912543743</v>
+        <v>1.2583780453206601</v>
       </c>
       <c r="G4" s="0">
-        <v>2.3707030314162498</v>
+        <v>2.370703156065936</v>
       </c>
       <c r="H4" s="0">
-        <v>6.5263047464024409</v>
+        <v>6.5263045999112155</v>
       </c>
       <c r="I4" s="0">
-        <v>3.5114132031278529</v>
+        <v>3.5114134292714567</v>
       </c>
       <c r="J4" s="0">
-        <v>1.765527783584655</v>
+        <v>1.765527751846999</v>
       </c>
       <c r="K4" s="0">
-        <v>1.6691623250900092</v>
+        <v>1.6691622787548694</v>
       </c>
       <c r="L4" s="0">
-        <v>1.5485356555140062</v>
+        <v>1.5485356216020518</v>
       </c>
       <c r="M4" s="0">
-        <v>2.2415335232846632</v>
+        <v>2.2415335055108359</v>
       </c>
       <c r="N4" s="0">
-        <v>2.4633466889271962</v>
+        <v>2.4633467041383397</v>
       </c>
       <c r="O4" s="0">
-        <v>1.4493390795822672</v>
+        <v>1.4493390875451944</v>
       </c>
       <c r="P4" s="0">
-        <v>1.2765867264458222</v>
+        <v>1.2765867426464319</v>
       </c>
       <c r="Q4" s="0">
-        <v>1.3023387625557605</v>
+        <v>1.3023389188300083</v>
       </c>
       <c r="R4" s="0">
-        <v>1.7625108771819744</v>
+        <v>1.7625108860269254</v>
       </c>
       <c r="S4" s="0">
-        <v>1.1252582806209131</v>
+        <v>1.1252583667680523</v>
       </c>
       <c r="T4" s="0">
-        <v>0.82201210050360563</v>
+        <v>0.82201210299048755</v>
       </c>
       <c r="U4" s="0">
-        <v>0.83802682212216939</v>
+        <v>0.83802682164702036</v>
       </c>
       <c r="V4" s="0">
-        <v>0.49552491434762735</v>
+        <v>0.49552491428702195</v>
       </c>
       <c r="W4" s="0">
-        <v>0.054537352789828922</v>
+        <v>0.054537352814066541</v>
       </c>
       <c r="X4" s="0">
         <v>0.23571173354711331</v>

</xml_diff>

<commit_message>
feat: mband noise further attempts and running experiments for power point
</commit_message>
<xml_diff>
--- a/Random/Matlab2025Files/SS/selected_algorithm_metrics.xlsx
+++ b/Random/Matlab2025Files/SS/selected_algorithm_metrics.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="80" uniqueCount="40">
   <si>
     <t>Algorithm</t>
   </si>
@@ -27,7 +27,19 @@
     <t>Estimated_noise</t>
   </si>
   <si>
-    <t>mband_normal</t>
+    <t>mband_noisetry_01</t>
+  </si>
+  <si>
+    <t>mband_noisetry_03</t>
+  </si>
+  <si>
+    <t>mband_noisetry_05</t>
+  </si>
+  <si>
+    <t>mband_noisetry_07</t>
+  </si>
+  <si>
+    <t>mband_noisetry_09</t>
   </si>
   <si>
     <t>File</t>
@@ -42,7 +54,19 @@
     <t>C:\Users\gabi\Documents\University\Uni2025\Investigation\PROJECT-25P85\results\EXP2\spectral\NOISE_ESTIMATION\enhanced_ESTIMATED_NOISE_standard_mode_BANDS4_SPACINGLINEAR_FRAME8ms.wav</t>
   </si>
   <si>
-    <t>C:\Users\gabi\Documents\University\Uni2025\Investigation\PROJECT-25P85\results\EXP2\spectral\NOISE_ESTIMATION\mband_normal_standard_mode_BANDS4_SPACINGLINEAR_FRAME8ms.wav</t>
+    <t>C:\Users\gabi\Documents\University\Uni2025\Investigation\PROJECT-25P85\results\EXP2\spectral\NOISE_ESTIMATION\mband_neural_vad_neural_guided_BANDS4_SPACINGLINEAR_FRAME8ms_NEURAL_W0.1.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\gabi\Documents\University\Uni2025\Investigation\PROJECT-25P85\results\EXP2\spectral\NOISE_ESTIMATION\mband_neural_vad_neural_guided_BANDS4_SPACINGLINEAR_FRAME8ms_NEURAL_W0.3.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\gabi\Documents\University\Uni2025\Investigation\PROJECT-25P85\results\EXP2\spectral\NOISE_ESTIMATION\mband_neural_vad_neural_guided_BANDS4_SPACINGLINEAR_FRAME8ms_NEURAL_W0.5.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\gabi\Documents\University\Uni2025\Investigation\PROJECT-25P85\results\EXP2\spectral\NOISE_ESTIMATION\mband_neural_vad_neural_guided_BANDS4_SPACINGLINEAR_FRAME8ms_NEURAL_W0.7.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\gabi\Documents\University\Uni2025\Investigation\PROJECT-25P85\results\EXP2\spectral\NOISE_ESTIMATION\mband_neural_vad_neural_guided_BANDS4_SPACINGLINEAR_FRAME8ms_NEURAL_W0.9.wav</t>
   </si>
   <si>
     <t>SNR</t>
@@ -154,13 +178,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="true"/>
+    <col min="1" max="1" width="17.54296875" customWidth="true"/>
     <col min="2" max="2" width="184.81640625" customWidth="true"/>
     <col min="3" max="3" width="11.453125" customWidth="true"/>
     <col min="4" max="4" width="13.08984375" customWidth="true"/>
@@ -191,73 +215,73 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
@@ -265,7 +289,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0">
         <v>5.0000005821993998</v>
@@ -339,7 +363,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0">
         <v>10.341197727994746</v>
@@ -413,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0">
         <v>7.6734063747941512</v>
@@ -487,72 +511,368 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0">
-        <v>7.673406372177908</v>
+        <v>7.704754856009604</v>
       </c>
       <c r="D5" s="0">
-        <v>2.1524493440773411</v>
+        <v>3.3462904559752613</v>
       </c>
       <c r="E5" s="0">
-        <v>88.185983819428614</v>
+        <v>66.024497435820607</v>
       </c>
       <c r="F5" s="0">
-        <v>1.2583780912543743</v>
+        <v>1.1556768900720593</v>
       </c>
       <c r="G5" s="0">
-        <v>2.3707030314162498</v>
+        <v>4.8330441143863947</v>
       </c>
       <c r="H5" s="0">
-        <v>6.5263047464024409</v>
+        <v>6.4641561894498256</v>
       </c>
       <c r="I5" s="0">
-        <v>3.5114132031278529</v>
+        <v>3.2655570396750266</v>
       </c>
       <c r="J5" s="0">
-        <v>1.765527783584655</v>
+        <v>1.6875575642659519</v>
       </c>
       <c r="K5" s="0">
-        <v>1.6691623250900092</v>
+        <v>1.5230599701597196</v>
       </c>
       <c r="L5" s="0">
-        <v>1.5485356555140062</v>
+        <v>1.3738670664190973</v>
       </c>
       <c r="M5" s="0">
-        <v>2.2415335232846632</v>
+        <v>1.861685810154585</v>
       </c>
       <c r="N5" s="0">
-        <v>2.4633466889271962</v>
+        <v>2.4671466761269221</v>
       </c>
       <c r="O5" s="0">
-        <v>1.4493390795822672</v>
+        <v>1.118705181794186</v>
       </c>
       <c r="P5" s="0">
-        <v>1.2765867264458222</v>
+        <v>1.3143859067555173</v>
       </c>
       <c r="Q5" s="0">
-        <v>1.3023387625557605</v>
+        <v>1.9912552546632791</v>
       </c>
       <c r="R5" s="0">
-        <v>1.7625108771819744</v>
+        <v>2.0109212801048337</v>
       </c>
       <c r="S5" s="0">
-        <v>1.1252582806209131</v>
+        <v>1.5430183344654736</v>
       </c>
       <c r="T5" s="0">
-        <v>0.82201210050360563</v>
+        <v>0.78524730472187798</v>
       </c>
       <c r="U5" s="0">
-        <v>0.83802682212216939</v>
+        <v>0.80486734112048897</v>
       </c>
       <c r="V5" s="0">
-        <v>0.49552491434762735</v>
+        <v>0.48618032404703787</v>
       </c>
       <c r="W5" s="0">
-        <v>0.054537352789828922</v>
+        <v>0.051653188045543641</v>
       </c>
       <c r="X5" s="0">
+        <v>0.23571173354711331</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0">
+        <v>7.704754856009604</v>
+      </c>
+      <c r="D6" s="0">
+        <v>3.3462904559752613</v>
+      </c>
+      <c r="E6" s="0">
+        <v>66.024497435820607</v>
+      </c>
+      <c r="F6" s="0">
+        <v>1.1556768900720593</v>
+      </c>
+      <c r="G6" s="0">
+        <v>4.8330441143863947</v>
+      </c>
+      <c r="H6" s="0">
+        <v>6.4641561894498256</v>
+      </c>
+      <c r="I6" s="0">
+        <v>3.2655570396750266</v>
+      </c>
+      <c r="J6" s="0">
+        <v>1.6875575642659519</v>
+      </c>
+      <c r="K6" s="0">
+        <v>1.5230599701597196</v>
+      </c>
+      <c r="L6" s="0">
+        <v>1.3738670664190973</v>
+      </c>
+      <c r="M6" s="0">
+        <v>1.861685810154585</v>
+      </c>
+      <c r="N6" s="0">
+        <v>2.4671466761269221</v>
+      </c>
+      <c r="O6" s="0">
+        <v>1.118705181794186</v>
+      </c>
+      <c r="P6" s="0">
+        <v>1.3143859067555173</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>1.9912552546632791</v>
+      </c>
+      <c r="R6" s="0">
+        <v>2.0109212801048337</v>
+      </c>
+      <c r="S6" s="0">
+        <v>1.5430183344654736</v>
+      </c>
+      <c r="T6" s="0">
+        <v>0.78524730472187798</v>
+      </c>
+      <c r="U6" s="0">
+        <v>0.80486734112048897</v>
+      </c>
+      <c r="V6" s="0">
+        <v>0.48618032404703787</v>
+      </c>
+      <c r="W6" s="0">
+        <v>0.051653188045543641</v>
+      </c>
+      <c r="X6" s="0">
+        <v>0.23571173354711331</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0">
+        <v>7.704754856009604</v>
+      </c>
+      <c r="D7" s="0">
+        <v>3.3462904559752613</v>
+      </c>
+      <c r="E7" s="0">
+        <v>66.024497435820607</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1.1556768900720593</v>
+      </c>
+      <c r="G7" s="0">
+        <v>4.8330441143863947</v>
+      </c>
+      <c r="H7" s="0">
+        <v>6.4641561894498256</v>
+      </c>
+      <c r="I7" s="0">
+        <v>3.2655570396750266</v>
+      </c>
+      <c r="J7" s="0">
+        <v>1.6875575642659519</v>
+      </c>
+      <c r="K7" s="0">
+        <v>1.5230599701597196</v>
+      </c>
+      <c r="L7" s="0">
+        <v>1.3738670664190973</v>
+      </c>
+      <c r="M7" s="0">
+        <v>1.861685810154585</v>
+      </c>
+      <c r="N7" s="0">
+        <v>2.4671466761269221</v>
+      </c>
+      <c r="O7" s="0">
+        <v>1.118705181794186</v>
+      </c>
+      <c r="P7" s="0">
+        <v>1.3143859067555173</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1.9912552546632791</v>
+      </c>
+      <c r="R7" s="0">
+        <v>2.0109212801048337</v>
+      </c>
+      <c r="S7" s="0">
+        <v>1.5430183344654736</v>
+      </c>
+      <c r="T7" s="0">
+        <v>0.78524730472187798</v>
+      </c>
+      <c r="U7" s="0">
+        <v>0.80486734112048897</v>
+      </c>
+      <c r="V7" s="0">
+        <v>0.48618032404703787</v>
+      </c>
+      <c r="W7" s="0">
+        <v>0.051653188045543641</v>
+      </c>
+      <c r="X7" s="0">
+        <v>0.23571173354711331</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0">
+        <v>7.704754856009604</v>
+      </c>
+      <c r="D8" s="0">
+        <v>3.3462904559752613</v>
+      </c>
+      <c r="E8" s="0">
+        <v>66.024497435820607</v>
+      </c>
+      <c r="F8" s="0">
+        <v>1.1556768900720593</v>
+      </c>
+      <c r="G8" s="0">
+        <v>4.8330441143863947</v>
+      </c>
+      <c r="H8" s="0">
+        <v>6.4641561894498256</v>
+      </c>
+      <c r="I8" s="0">
+        <v>3.2655570396750266</v>
+      </c>
+      <c r="J8" s="0">
+        <v>1.6875575642659519</v>
+      </c>
+      <c r="K8" s="0">
+        <v>1.5230599701597196</v>
+      </c>
+      <c r="L8" s="0">
+        <v>1.3738670664190973</v>
+      </c>
+      <c r="M8" s="0">
+        <v>1.861685810154585</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2.4671466761269221</v>
+      </c>
+      <c r="O8" s="0">
+        <v>1.118705181794186</v>
+      </c>
+      <c r="P8" s="0">
+        <v>1.3143859067555173</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>1.9912552546632791</v>
+      </c>
+      <c r="R8" s="0">
+        <v>2.0109212801048337</v>
+      </c>
+      <c r="S8" s="0">
+        <v>1.5430183344654736</v>
+      </c>
+      <c r="T8" s="0">
+        <v>0.78524730472187798</v>
+      </c>
+      <c r="U8" s="0">
+        <v>0.80486734112048897</v>
+      </c>
+      <c r="V8" s="0">
+        <v>0.48618032404703787</v>
+      </c>
+      <c r="W8" s="0">
+        <v>0.051653188045543641</v>
+      </c>
+      <c r="X8" s="0">
+        <v>0.23571173354711331</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0">
+        <v>7.704754856009604</v>
+      </c>
+      <c r="D9" s="0">
+        <v>3.3462904559752613</v>
+      </c>
+      <c r="E9" s="0">
+        <v>66.024497435820607</v>
+      </c>
+      <c r="F9" s="0">
+        <v>1.1556768900720593</v>
+      </c>
+      <c r="G9" s="0">
+        <v>4.8330441143863947</v>
+      </c>
+      <c r="H9" s="0">
+        <v>6.4641561894498256</v>
+      </c>
+      <c r="I9" s="0">
+        <v>3.2655570396750266</v>
+      </c>
+      <c r="J9" s="0">
+        <v>1.6875575642659519</v>
+      </c>
+      <c r="K9" s="0">
+        <v>1.5230599701597196</v>
+      </c>
+      <c r="L9" s="0">
+        <v>1.3738670664190973</v>
+      </c>
+      <c r="M9" s="0">
+        <v>1.861685810154585</v>
+      </c>
+      <c r="N9" s="0">
+        <v>2.4671466761269221</v>
+      </c>
+      <c r="O9" s="0">
+        <v>1.118705181794186</v>
+      </c>
+      <c r="P9" s="0">
+        <v>1.3143859067555173</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>1.9912552546632791</v>
+      </c>
+      <c r="R9" s="0">
+        <v>2.0109212801048337</v>
+      </c>
+      <c r="S9" s="0">
+        <v>1.5430183344654736</v>
+      </c>
+      <c r="T9" s="0">
+        <v>0.78524730472187798</v>
+      </c>
+      <c r="U9" s="0">
+        <v>0.80486734112048897</v>
+      </c>
+      <c r="V9" s="0">
+        <v>0.48618032404703787</v>
+      </c>
+      <c r="W9" s="0">
+        <v>0.051653188045543641</v>
+      </c>
+      <c r="X9" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>

</xml_diff>